<commit_message>
automação de abrir a página do wats
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calebeh1000_00\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B88B6322-AD74-4505-810E-3B4CA71DEAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A01A5F-17CD-4BD5-A416-0F7D4F243D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0A187E6-EE1C-41BC-9A03-F3FFDA68EA2A}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Calebe</t>
   </si>
   <si>
-    <t>55489996631726</t>
-  </si>
-  <si>
     <t>Karen</t>
   </si>
   <si>
@@ -54,13 +51,19 @@
   </si>
   <si>
     <t>5548988378444</t>
+  </si>
+  <si>
+    <t>05/10/2025</t>
+  </si>
+  <si>
+    <t>5548999663176</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,12 +107,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,53 +450,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99D5409-0930-4CCF-B826-8DCA9F8DECB7}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3">
         <v>45935</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
-        <v>45935</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>45935</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 #PÚBLICO#</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6c93f401-da26-4519-94e2-7a6b9f1a3c5d}" enabled="1" method="Privileged" siteId="{ba297f1d-f19e-425f-ad15-7b419df80522}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>